<commit_message>
diferencia entre stock y demanda
</commit_message>
<xml_diff>
--- a/Demandas_y_Asignacion.xlsx
+++ b/Demandas_y_Asignacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="29">
   <si>
     <t>Stock</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Demanda</t>
+  </si>
+  <si>
+    <t>Diferencia</t>
   </si>
 </sst>
 </file>
@@ -164,11 +167,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,7 +183,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -473,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L27"/>
+  <dimension ref="B1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -487,54 +524,54 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="16" customWidth="1"/>
     <col min="7" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
-      <c r="D1" s="4" t="s">
+    <row r="1" spans="2:11">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="1"/>
-      <c r="K1" s="5" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="J1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="2:12">
-      <c r="B2" s="2" t="s">
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="2:11">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:11">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -547,14 +584,18 @@
       <c r="E3">
         <v>9000</v>
       </c>
-      <c r="K3" t="s">
+      <c r="I3">
+        <f>D3-E3</f>
+        <v>10800</v>
+      </c>
+      <c r="J3" t="s">
         <v>2</v>
       </c>
-      <c r="L3">
+      <c r="K3">
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:11">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -567,14 +608,18 @@
       <c r="E4">
         <v>193536</v>
       </c>
-      <c r="K4" t="s">
+      <c r="I4">
+        <f t="shared" ref="I4:I13" si="0">D4-E4</f>
+        <v>-134784</v>
+      </c>
+      <c r="J4" t="s">
         <v>3</v>
       </c>
-      <c r="L4">
+      <c r="K4">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -587,14 +632,18 @@
       <c r="E5">
         <v>1200</v>
       </c>
-      <c r="K5" t="s">
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>2400</v>
+      </c>
+      <c r="J5" t="s">
         <v>4</v>
       </c>
-      <c r="L5">
+      <c r="K5">
         <v>9000</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:11">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -607,14 +656,18 @@
       <c r="E6">
         <v>69120</v>
       </c>
-      <c r="K6" t="s">
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>-48960</v>
+      </c>
+      <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="L6">
+      <c r="K6">
         <v>9600</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:11">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -627,14 +680,18 @@
       <c r="E7">
         <v>1848</v>
       </c>
-      <c r="K7" t="s">
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>2688</v>
+      </c>
+      <c r="J7" t="s">
         <v>6</v>
       </c>
-      <c r="L7">
+      <c r="K7">
         <v>580</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:11">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -647,14 +704,18 @@
       <c r="E8">
         <v>34560</v>
       </c>
-      <c r="K8" t="s">
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>-24840</v>
+      </c>
+      <c r="J8" t="s">
         <v>7</v>
       </c>
-      <c r="L8">
+      <c r="K8">
         <v>2700</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:11">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -667,14 +728,18 @@
       <c r="E9">
         <v>4800</v>
       </c>
-      <c r="K9" t="s">
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>-2400</v>
+      </c>
+      <c r="J9" t="s">
         <v>8</v>
       </c>
-      <c r="L9">
+      <c r="K9">
         <v>7500</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:11">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -687,14 +752,18 @@
       <c r="E10">
         <v>65400</v>
       </c>
-      <c r="K10" t="s">
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>-11640</v>
+      </c>
+      <c r="J10" t="s">
         <v>9</v>
       </c>
-      <c r="L10">
+      <c r="K10">
         <v>7500</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:11">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -707,14 +776,18 @@
       <c r="E11">
         <v>32400</v>
       </c>
-      <c r="K11" t="s">
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>25200</v>
+      </c>
+      <c r="J11" t="s">
         <v>10</v>
       </c>
-      <c r="L11">
+      <c r="K11">
         <v>10000</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:11">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -727,14 +800,18 @@
       <c r="E12">
         <v>79200</v>
       </c>
-      <c r="K12" t="s">
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>-7200</v>
+      </c>
+      <c r="J12" t="s">
         <v>11</v>
       </c>
-      <c r="L12">
+      <c r="K12">
         <v>9500</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:11">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -747,44 +824,48 @@
       <c r="E13">
         <v>10800</v>
       </c>
-      <c r="K13" t="s">
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>-5400</v>
+      </c>
+      <c r="J13" t="s">
         <v>12</v>
       </c>
-      <c r="L13">
+      <c r="K13">
         <v>9000</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
-      <c r="D15" s="3" t="s">
+    <row r="15" spans="2:11">
+      <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="2:12">
-      <c r="B16" s="2" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:11">
       <c r="B17" t="s">
         <v>2</v>
       </c>
@@ -797,14 +878,14 @@
       <c r="E17">
         <v>9000</v>
       </c>
-      <c r="K17" t="s">
+      <c r="J17" t="s">
         <v>2</v>
       </c>
-      <c r="L17">
+      <c r="K17">
         <v>20000</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:11">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -817,14 +898,14 @@
       <c r="E18">
         <v>17280</v>
       </c>
-      <c r="K18" t="s">
+      <c r="J18" t="s">
         <v>3</v>
       </c>
-      <c r="L18">
+      <c r="K18">
         <v>10000</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:11">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -837,14 +918,14 @@
       <c r="E19">
         <v>0</v>
       </c>
-      <c r="K19" t="s">
+      <c r="J19" t="s">
         <v>4</v>
       </c>
-      <c r="L19">
+      <c r="K19">
         <v>9000</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:11">
       <c r="B20" t="s">
         <v>5</v>
       </c>
@@ -857,14 +938,14 @@
       <c r="E20">
         <v>9600</v>
       </c>
-      <c r="K20" t="s">
+      <c r="J20" t="s">
         <v>5</v>
       </c>
-      <c r="L20">
+      <c r="K20">
         <v>9600</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:11">
       <c r="B21" t="s">
         <v>6</v>
       </c>
@@ -877,14 +958,14 @@
       <c r="E21">
         <v>0</v>
       </c>
-      <c r="K21" t="s">
+      <c r="J21" t="s">
         <v>6</v>
       </c>
-      <c r="L21">
+      <c r="K21">
         <v>580</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:11">
       <c r="B22" t="s">
         <v>7</v>
       </c>
@@ -897,14 +978,14 @@
       <c r="E22">
         <v>4320</v>
       </c>
-      <c r="K22" t="s">
+      <c r="J22" t="s">
         <v>7</v>
       </c>
-      <c r="L22">
+      <c r="K22">
         <v>2700</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:11">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -917,14 +998,14 @@
       <c r="E23">
         <v>0</v>
       </c>
-      <c r="K23" t="s">
+      <c r="J23" t="s">
         <v>8</v>
       </c>
-      <c r="L23">
+      <c r="K23">
         <v>7500</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:11">
       <c r="B24" t="s">
         <v>9</v>
       </c>
@@ -937,14 +1018,14 @@
       <c r="E24">
         <v>2400</v>
       </c>
-      <c r="K24" t="s">
+      <c r="J24" t="s">
         <v>9</v>
       </c>
-      <c r="L24">
+      <c r="K24">
         <v>7500</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:11">
       <c r="B25" t="s">
         <v>10</v>
       </c>
@@ -957,14 +1038,14 @@
       <c r="E25">
         <v>0</v>
       </c>
-      <c r="K25" t="s">
+      <c r="J25" t="s">
         <v>10</v>
       </c>
-      <c r="L25">
+      <c r="K25">
         <v>10000</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:11">
       <c r="B26" t="s">
         <v>11</v>
       </c>
@@ -977,14 +1058,14 @@
       <c r="E26">
         <v>10800</v>
       </c>
-      <c r="K26" t="s">
+      <c r="J26" t="s">
         <v>11</v>
       </c>
-      <c r="L26">
+      <c r="K26">
         <v>9500</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="2:11">
       <c r="B27" t="s">
         <v>12</v>
       </c>
@@ -997,10 +1078,10 @@
       <c r="E27">
         <v>2400</v>
       </c>
-      <c r="K27" t="s">
+      <c r="J27" t="s">
         <v>12</v>
       </c>
-      <c r="L27">
+      <c r="K27">
         <v>9000</v>
       </c>
     </row>
@@ -1008,8 +1089,16 @@
   <mergeCells count="3">
     <mergeCell ref="D15:H15"/>
     <mergeCell ref="D1:H1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
+  <conditionalFormatting sqref="I3:I13">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1038,53 +1127,53 @@
       </c>
     </row>
     <row r="3" spans="2:12">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>